<commit_message>
SSDM-12286 Fixed letter case inconsistencies.
</commit_message>
<xml_diff>
--- a/openbis/sourceTest/java/ch/ethz/sis/openbis/generic/server/xls/export/resources/export-data-set-type.xlsx
+++ b/openbis/sourceTest/java/ch/ethz/sis/openbis/generic/server/xls/export/resources/export-data-set-type.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vkovtun/Work/Projects/openBIS/sissource/openbis/openbis/sourceTest/java/ch/ethz/sis/openbis/generic/server/xls/export/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4AFDF4A-973F-874C-9757-ABBDE1B36EFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A15C7C9-FF8A-B746-81B7-A26B4A095F76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7340" yWindow="2700" windowWidth="27640" windowHeight="16940" xr2:uid="{75C30B8F-E590-0942-81AA-3FAD886CC976}"/>
+    <workbookView xWindow="1460" yWindow="1060" windowWidth="27340" windowHeight="16940" xr2:uid="{75C30B8F-E590-0942-81AA-3FAD886CC976}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
@@ -68,9 +68,6 @@
     <t>Data type</t>
   </si>
   <si>
-    <t>Vocabulary Code</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
@@ -126,6 +123,9 @@
   </si>
   <si>
     <t>Comments</t>
+  </si>
+  <si>
+    <t>Vocabulary code</t>
   </si>
 </sst>
 </file>
@@ -491,14 +491,14 @@
   <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD8"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
@@ -517,7 +517,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>5</v>
@@ -546,16 +546,16 @@
         <v>10</v>
       </c>
       <c r="H4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="J4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="K4" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
@@ -563,28 +563,28 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>16</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>4</v>
       </c>
       <c r="E5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="G5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G5" s="2" t="s">
-        <v>19</v>
-      </c>
       <c r="H5" s="2" t="s">
         <v>5</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J5" s="2" t="s">
         <v>5</v>
@@ -598,31 +598,31 @@
         <v>3</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>4</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J6" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>21</v>
       </c>
       <c r="K6" s="2" t="s">
         <v>5</v>
@@ -633,26 +633,26 @@
         <v>3</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I7" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>27</v>
       </c>
       <c r="J7" s="2" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
SSDM-13163 Renamed "DATA_SET_TYPE" to the correct "DATASET_TYPE" in export.
</commit_message>
<xml_diff>
--- a/openbis/sourceTest/java/ch/ethz/sis/openbis/generic/server/xls/export/resources/export-data-set-type.xlsx
+++ b/openbis/sourceTest/java/ch/ethz/sis/openbis/generic/server/xls/export/resources/export-data-set-type.xlsx
@@ -22,7 +22,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="31">
   <si>
-    <t xml:space="preserve">DATA_SET_TYPE</t>
+    <t xml:space="preserve">DATASET_TYPE</t>
   </si>
   <si>
     <t xml:space="preserve">Version</t>
@@ -234,10 +234,10 @@
   <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">

</xml_diff>